<commit_message>
cambio en la matric de excel
</commit_message>
<xml_diff>
--- a/La Matrix.xlsx
+++ b/La Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="67">
   <si>
     <t>L</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>AS15: AGREGAR AL STRING IGUAL</t>
+  </si>
+  <si>
+    <t>error: rangos de constantes y cantidad de caracteres de identificador</t>
+  </si>
+  <si>
+    <t>cometario multilinea llega al final del archivo entonces error</t>
   </si>
 </sst>
 </file>
@@ -483,6 +489,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,366 +517,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1194,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,7 +954,7 @@
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1890,13 +1546,13 @@
     </row>
     <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12"/>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1921,12 +1577,12 @@
       <c r="B13" s="17">
         <v>0</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1951,12 +1607,12 @@
       <c r="B14" s="18">
         <v>1</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1981,12 +1637,12 @@
       <c r="B15" s="18">
         <v>2</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2011,103 +1667,113 @@
       <c r="B16" s="18">
         <v>3</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="18">
         <v>4</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="18">
         <v>5</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="18">
         <v>6</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="19">
         <v>7</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>51</v>
       </c>
@@ -2155,10 +1821,10 @@
     <mergeCell ref="C16:F16"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:X10">
-    <cfRule type="containsText" dxfId="51" priority="2" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",C3)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"E"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Soporte de lectura de matriz de acciones semánticas
</commit_message>
<xml_diff>
--- a/La Matrix.xlsx
+++ b/La Matrix.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Desktop\LeCompilateurMagnifique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pancho\Documents\FACULTAD\4° Año 2° Cuatrimestre\Diseño de Compiladores\Le Compilateur Magnifique\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8352"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -483,6 +483,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,366 +514,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1194,38 +847,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="9" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="7.21875" customWidth="1"/>
-    <col min="12" max="12" width="8.21875" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" customWidth="1"/>
-    <col min="16" max="16" width="9.77734375" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
     <col min="19" max="19" width="8" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" customWidth="1"/>
     <col min="21" max="21" width="8" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" customWidth="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.109375" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="X1" s="10"/>
     </row>
-    <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9"/>
       <c r="C2" s="6" t="s">
         <v>0</v>
@@ -1294,11 +947,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1365,7 +1018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -1436,7 +1089,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1507,7 +1160,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -1578,7 +1231,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -1649,7 +1302,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -1720,7 +1373,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -1791,7 +1444,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>7</v>
       </c>
@@ -1862,7 +1515,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
@@ -1870,7 +1523,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="21"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1888,15 +1541,15 @@
       <c r="W11" s="1"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1916,17 +1569,17 @@
       <c r="W12" s="1"/>
       <c r="X12" s="12"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="17">
         <v>0</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1946,17 +1599,17 @@
       <c r="W13" s="1"/>
       <c r="X13" s="12"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="18">
         <v>1</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1976,17 +1629,17 @@
       <c r="W14" s="1"/>
       <c r="X14" s="12"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="18">
         <v>2</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2007,137 +1660,137 @@
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="18">
         <v>3</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="18">
         <v>4</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="18">
         <v>5</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="18">
         <v>6</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="19">
         <v>7</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>64</v>
       </c>
@@ -2155,10 +1808,10 @@
     <mergeCell ref="C16:F16"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:X10">
-    <cfRule type="containsText" dxfId="51" priority="2" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",C3)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"E"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Se acomodó un poco el código
</commit_message>
<xml_diff>
--- a/La Matrix.xlsx
+++ b/La Matrix.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Desktop\LeCompilateurMagnifique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pancho\Documents\FACULTAD\4° Año 2° Cuatrimestre\Diseño de Compiladores\Le Compilateur Magnifique\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8352"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="70">
   <si>
     <t>L</t>
   </si>
@@ -225,13 +226,22 @@
   </si>
   <si>
     <t>cometario multilinea llega al final del archivo entonces error</t>
+  </si>
+  <si>
+    <t>COLUMNA -&gt;</t>
+  </si>
+  <si>
+    <t>ERROR -&gt; -1</t>
+  </si>
+  <si>
+    <t>FINAL -&gt; -2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +264,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -433,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,7 +488,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -519,6 +544,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,38 +879,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="9" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="7.21875" customWidth="1"/>
-    <col min="12" max="12" width="8.21875" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" customWidth="1"/>
-    <col min="16" max="16" width="9.77734375" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
     <col min="19" max="19" width="8" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" customWidth="1"/>
     <col min="21" max="21" width="8" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" customWidth="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.109375" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="X1" s="10"/>
-    </row>
-    <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="30">
+        <v>0</v>
+      </c>
+      <c r="D1" s="30">
+        <v>1</v>
+      </c>
+      <c r="E1" s="30">
+        <v>2</v>
+      </c>
+      <c r="F1" s="30">
+        <v>3</v>
+      </c>
+      <c r="G1" s="30">
+        <v>4</v>
+      </c>
+      <c r="H1" s="30">
+        <v>5</v>
+      </c>
+      <c r="I1" s="30">
+        <v>6</v>
+      </c>
+      <c r="J1" s="30">
+        <v>7</v>
+      </c>
+      <c r="K1" s="30">
+        <v>8</v>
+      </c>
+      <c r="L1" s="30">
+        <v>9</v>
+      </c>
+      <c r="M1" s="30">
+        <v>10</v>
+      </c>
+      <c r="N1" s="30">
+        <v>11</v>
+      </c>
+      <c r="O1" s="30">
+        <v>12</v>
+      </c>
+      <c r="P1" s="30">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="30">
+        <v>14</v>
+      </c>
+      <c r="R1" s="30">
+        <v>15</v>
+      </c>
+      <c r="S1" s="30">
+        <v>16</v>
+      </c>
+      <c r="T1" s="30">
+        <v>17</v>
+      </c>
+      <c r="U1" s="30">
+        <v>18</v>
+      </c>
+      <c r="V1" s="30">
+        <v>19</v>
+      </c>
+      <c r="W1" s="30">
+        <v>20</v>
+      </c>
+      <c r="X1" s="30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9"/>
       <c r="C2" s="6" t="s">
         <v>0</v>
@@ -913,10 +1010,10 @@
       <c r="L2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="O2" s="7" t="s">
@@ -946,15 +1043,15 @@
       <c r="W2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="X2" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1017,437 +1114,437 @@
       <c r="W3" s="2">
         <v>0</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="Q4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="S4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="T4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="U4" s="20" t="s">
+      <c r="U4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="V4" s="20" t="s">
+      <c r="V4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="20" t="s">
+      <c r="W4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="X4" s="15" t="s">
+      <c r="X4" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="20" t="s">
+      <c r="D5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="T5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="U5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="V5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="W5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="X5" s="15" t="s">
+      <c r="K5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="X5" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="20" t="s">
+      <c r="D6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="U6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="V6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="W6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="X6" s="15" t="s">
+      <c r="K6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="U6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="20" t="s">
+      <c r="D7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="R7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="S7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="T7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="U7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="V7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="W7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="X7" s="15" t="s">
+      <c r="K7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="N8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="Q8" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R8" s="20" t="s">
+      <c r="R8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="20" t="s">
+      <c r="S8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="U8" s="20" t="s">
+      <c r="U8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="V8" s="20" t="s">
+      <c r="V8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="W8" s="20" t="s">
+      <c r="W8" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="X8" s="15" t="s">
+      <c r="X8" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>6</v>
       </c>
       <c r="C9" s="3">
         <v>6</v>
       </c>
-      <c r="D9" s="14">
-        <v>6</v>
-      </c>
-      <c r="E9" s="14">
-        <v>6</v>
-      </c>
-      <c r="F9" s="14">
-        <v>6</v>
-      </c>
-      <c r="G9" s="14">
+      <c r="D9" s="13">
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <v>6</v>
+      </c>
+      <c r="F9" s="13">
+        <v>6</v>
+      </c>
+      <c r="G9" s="13">
         <v>0</v>
       </c>
-      <c r="H9" s="14">
-        <v>6</v>
-      </c>
-      <c r="I9" s="14">
-        <v>6</v>
-      </c>
-      <c r="J9" s="14">
-        <v>6</v>
-      </c>
-      <c r="K9" s="14">
-        <v>6</v>
-      </c>
-      <c r="L9" s="14">
-        <v>6</v>
-      </c>
-      <c r="M9" s="14">
-        <v>6</v>
-      </c>
-      <c r="N9" s="14">
-        <v>6</v>
-      </c>
-      <c r="O9" s="14">
-        <v>6</v>
-      </c>
-      <c r="P9" s="20">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="14">
-        <v>6</v>
-      </c>
-      <c r="R9" s="14">
-        <v>6</v>
-      </c>
-      <c r="S9" s="14">
-        <v>6</v>
-      </c>
-      <c r="T9" s="14">
-        <v>6</v>
-      </c>
-      <c r="U9" s="14">
-        <v>6</v>
-      </c>
-      <c r="V9" s="14">
-        <v>6</v>
-      </c>
-      <c r="W9" s="14">
-        <v>6</v>
-      </c>
-      <c r="X9" s="15" t="s">
+      <c r="H9" s="13">
+        <v>6</v>
+      </c>
+      <c r="I9" s="13">
+        <v>6</v>
+      </c>
+      <c r="J9" s="13">
+        <v>6</v>
+      </c>
+      <c r="K9" s="13">
+        <v>6</v>
+      </c>
+      <c r="L9" s="13">
+        <v>6</v>
+      </c>
+      <c r="M9" s="13">
+        <v>6</v>
+      </c>
+      <c r="N9" s="13">
+        <v>6</v>
+      </c>
+      <c r="O9" s="13">
+        <v>6</v>
+      </c>
+      <c r="P9" s="19">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>6</v>
+      </c>
+      <c r="R9" s="13">
+        <v>6</v>
+      </c>
+      <c r="S9" s="13">
+        <v>6</v>
+      </c>
+      <c r="T9" s="13">
+        <v>6</v>
+      </c>
+      <c r="U9" s="13">
+        <v>6</v>
+      </c>
+      <c r="V9" s="13">
+        <v>6</v>
+      </c>
+      <c r="W9" s="13">
+        <v>6</v>
+      </c>
+      <c r="X9" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>7</v>
       </c>
@@ -1514,12 +1611,12 @@
       <c r="W10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="X10" s="15" t="s">
+      <c r="X10" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1531,8 +1628,8 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -1542,25 +1639,25 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
-      <c r="X11" s="13"/>
-    </row>
-    <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
-      <c r="B12" s="26" t="s">
+      <c r="X11" s="12"/>
+    </row>
+    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1570,27 +1667,29 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="12"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="17">
+      <c r="X12" s="11"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="16">
         <v>0</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -1600,27 +1699,29 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
-      <c r="X13" s="12"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18">
+      <c r="X13" s="11"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="17">
         <v>1</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -1630,180 +1731,181 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="12"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18">
+      <c r="X14" s="11"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="17">
         <v>2</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="20"/>
+      <c r="S15" s="19"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B16" s="18">
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="17">
         <v>3</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="17">
         <v>4</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="18">
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="17">
         <v>5</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="18">
-        <v>6</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="17">
+        <v>6</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-    </row>
-    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="19">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18">
         <v>7</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="25"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="H32" s="31"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>64</v>
       </c>

</xml_diff>